<commit_message>
Update core switch configuration to include VLAN200, the guest network
</commit_message>
<xml_diff>
--- a/network/core-switch-configuration-sg1016de.xlsx
+++ b/network/core-switch-configuration-sg1016de.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacib\Documents\Prog\FRC\JMS\network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEAB7F1-209C-4498-A50C-F421D37178AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E73CECA4-ABC7-4164-A5FD-52D1CC2DAAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7C68B60C-30E7-4557-8A22-4725DAB8D7D7}"/>
+    <workbookView xWindow="27645" yWindow="1575" windowWidth="34635" windowHeight="18390" xr2:uid="{7C68B60C-30E7-4557-8A22-4725DAB8D7D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>RED 3</t>
   </si>
@@ -86,21 +86,12 @@
     <t>10 / 20 / 30</t>
   </si>
   <si>
-    <t>10,20,30,40,50,60,100</t>
-  </si>
-  <si>
-    <t>10,20,30,100</t>
-  </si>
-  <si>
     <t>RED 1 / 2/ 3</t>
   </si>
   <si>
     <t>40 / 50 / 60</t>
   </si>
   <si>
-    <t>40,50,60,100</t>
-  </si>
-  <si>
     <t>Tagged in case of aggregating switch at alliance station</t>
   </si>
   <si>
@@ -113,13 +104,13 @@
     <t>JMS Core Switch Configuration (SG1016DE)</t>
   </si>
   <si>
-    <t>10,20,30,40,50,60,99,100</t>
-  </si>
-  <si>
     <t>SWITCH MGMT</t>
   </si>
   <si>
     <t>admin:jmsR0cks  (192.168.0.1)</t>
+  </si>
+  <si>
+    <t>1,10,20,30,40,50,60,99,100,200</t>
   </si>
 </sst>
 </file>
@@ -270,14 +261,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,7 +587,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,30 +597,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
+      <c r="B1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
     </row>
     <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
+      <c r="B2" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="10"/>
@@ -674,10 +665,10 @@
     </row>
     <row r="5" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>26</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>7</v>
@@ -706,7 +697,7 @@
     </row>
     <row r="6" spans="1:12" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>9</v>
@@ -782,7 +773,7 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -793,7 +784,7 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -804,7 +795,7 @@
         <v>99</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -815,7 +806,7 @@
         <v>100</v>
       </c>
       <c r="E13" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -826,24 +817,24 @@
         <v>15</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>